<commit_message>
need to add git ignore as well to this page
</commit_message>
<xml_diff>
--- a/dev/enchantMinDmg.xlsx
+++ b/dev/enchantMinDmg.xlsx
@@ -1,19 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\WebstormProjects\diablo2-notes\dev\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FACE5A6-FCA9-4625-B3AC-F757E9528644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>lvl</t>
+  </si>
+  <si>
+    <t>minDmg</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -50,7 +69,1509 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.5401456555395306E-2"/>
+          <c:y val="0.11140033394765761"/>
+          <c:w val="0.92352733554146316"/>
+          <c:h val="0.82818794687265718"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>minDmg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>sheet1!$A$2:$A$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>sheet1!$B$2:$B$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="99"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>46.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>57.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>68.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>79.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>94.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>109.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>124.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>143.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>162.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>181.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>200.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>219.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>238.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>257.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>276.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>286</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>295.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>314.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>333.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>343</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>352.5</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>362</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>371.5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>381</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>390.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>409.5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>428.5</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>438</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>447.5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>457</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>466.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>476</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>485.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>504.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>514</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>523.5</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>533</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>542.5</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>552</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>561.5</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>571</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>580.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>599.5</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>609</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>618.5</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>628</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>637.5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>647</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>656.5</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>666</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>675.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>685</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>694.5</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>704</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>713.5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>723</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>732.5</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>742</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>751.5</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>761</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>770.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>789.5</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C9E9-415A-B8A5-1741C6FBAF9A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="639248136"/>
+        <c:axId val="639252400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="639248136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="639252400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="639252400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="639248136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>206429</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>72914</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>392167</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>193784</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2348A75D-89E8-4395-9240-487C92C3F7DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -374,21 +1895,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>lvl</v>
-      </c>
-      <c r="B1" t="str">
-        <v>minDmg</v>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -396,7 +1920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -404,7 +1928,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -412,7 +1936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -420,7 +1944,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -428,7 +1952,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -436,7 +1960,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -444,7 +1968,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -452,7 +1976,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -460,7 +1984,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -468,7 +1992,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -476,7 +2000,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -484,7 +2008,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -492,7 +2016,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -500,7 +2024,7 @@
         <v>39.5</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -508,7 +2032,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -516,7 +2040,7 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -524,7 +2048,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -532,7 +2056,7 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -540,7 +2064,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -548,7 +2072,7 @@
         <v>68.5</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -556,7 +2080,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -564,7 +2088,7 @@
         <v>79.5</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -572,7 +2096,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -580,7 +2104,7 @@
         <v>94.5</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -588,7 +2112,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -596,7 +2120,7 @@
         <v>109.5</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -604,7 +2128,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -612,7 +2136,7 @@
         <v>124.5</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -620,7 +2144,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -628,7 +2152,7 @@
         <v>143.5</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -636,7 +2160,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -644,7 +2168,7 @@
         <v>162.5</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -652,7 +2176,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -660,7 +2184,7 @@
         <v>181.5</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -668,7 +2192,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -676,7 +2200,7 @@
         <v>200.5</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -684,7 +2208,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -692,7 +2216,7 @@
         <v>219.5</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -700,7 +2224,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -708,7 +2232,7 @@
         <v>238.5</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -716,7 +2240,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -724,7 +2248,7 @@
         <v>257.5</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -732,7 +2256,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -740,7 +2264,7 @@
         <v>276.5</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -748,7 +2272,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -756,7 +2280,7 @@
         <v>295.5</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -764,7 +2288,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -772,7 +2296,7 @@
         <v>314.5</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -780,7 +2304,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -788,7 +2312,7 @@
         <v>333.5</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -796,7 +2320,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -804,7 +2328,7 @@
         <v>352.5</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -812,7 +2336,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -820,7 +2344,7 @@
         <v>371.5</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -828,7 +2352,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -836,7 +2360,7 @@
         <v>390.5</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -844,7 +2368,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -852,7 +2376,7 @@
         <v>409.5</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -860,7 +2384,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -868,7 +2392,7 @@
         <v>428.5</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -876,7 +2400,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -884,7 +2408,7 @@
         <v>447.5</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -892,7 +2416,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -900,7 +2424,7 @@
         <v>466.5</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -908,7 +2432,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -916,7 +2440,7 @@
         <v>485.5</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -924,7 +2448,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -932,7 +2456,7 @@
         <v>504.5</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -940,7 +2464,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -948,7 +2472,7 @@
         <v>523.5</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -956,7 +2480,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -964,7 +2488,7 @@
         <v>542.5</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -972,7 +2496,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -980,7 +2504,7 @@
         <v>561.5</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -988,7 +2512,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -996,7 +2520,7 @@
         <v>580.5</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1004,7 +2528,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1012,7 +2536,7 @@
         <v>599.5</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1020,7 +2544,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1028,7 +2552,7 @@
         <v>618.5</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -1036,7 +2560,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -1044,7 +2568,7 @@
         <v>637.5</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -1052,7 +2576,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -1060,7 +2584,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -1068,7 +2592,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -1076,7 +2600,7 @@
         <v>675.5</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -1084,7 +2608,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -1092,7 +2616,7 @@
         <v>694.5</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -1100,7 +2624,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -1108,7 +2632,7 @@
         <v>713.5</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -1116,7 +2640,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -1124,7 +2648,7 @@
         <v>732.5</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -1132,7 +2656,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -1140,7 +2664,7 @@
         <v>751.5</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -1148,7 +2672,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -1156,7 +2680,7 @@
         <v>770.5</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -1164,7 +2688,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -1172,7 +2696,7 @@
         <v>789.5</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -1181,8 +2705,10 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B100"/>
+    <ignoredError sqref="A1:B100" numberStoredAsText="1"/>
   </ignoredErrors>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>